<commit_message>
Update with latest code
</commit_message>
<xml_diff>
--- a/DataForTest/PLO_Civil.xlsx
+++ b/DataForTest/PLO_Civil.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="28623"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="28827"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\phans\Desktop\DataForTest\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{02C0DD1F-A523-4AD6-A76F-BB865B92F308}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CB2DC682-82BD-4D17-832D-12800C4A90E8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="732" yWindow="732" windowWidth="14196" windowHeight="11316" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="10020" yWindow="0" windowWidth="11472" windowHeight="12240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -64,9 +64,6 @@
     <t>สามารถแสดงว่ามีความรู้และความเข้าใจหลักการทางวิศวกรรมและการบริหารงาน และสามารถประยุกต์ใช้หลักการบริหารในงานของตน ในฐานะผู้ร่วมทีมและผู้นำทีมเพื่อบริหารจัดการโครงการวิศวกรรมที่มีสภาพแวดล้อมการทำงานที่มีความหลากหลายสาขาวิชาชีพ สามารถแสดงออกถึงความมีวิสัยทัศน์ด้านการลงทุนและการเป็นผู้ประกอบการ</t>
   </si>
   <si>
-    <t>ตระหนักและเห็นความจำเป็นของการพัฒนาตนเองอย่างต่อเนื่อง มีการเตรียมตัวเพื่อให้สามารถปฏิบัติงานได้โดยลำพังและสามารถเรียนรู้ตลอดชีพเมื่อมีการเปลี่ยนแปลงทางด้านเทคโนโลยีและวิศวกรรม</t>
-  </si>
-  <si>
     <t>Able to apply knowledge in mathematics, science, basic engineering, and specialized engineering knowledge to solve and find solutions for complex engineering problems.</t>
   </si>
   <si>
@@ -100,43 +97,46 @@
     <t>Able to demonstrate knowledge and understanding of engineering and management principles and apply them in their work as team members or leaders, managing engineering projects in diverse environments with a vision for investment and entrepreneurship.</t>
   </si>
   <si>
-    <t>Recognize the need for continuous self-development, be prepared for independent work, and engage in lifelong learning in response to technological and engineering changes.</t>
-  </si>
-  <si>
-    <t>PLO 1</t>
-  </si>
-  <si>
-    <t>PLO 2</t>
-  </si>
-  <si>
-    <t>PLO 3</t>
-  </si>
-  <si>
-    <t>PLO 4</t>
-  </si>
-  <si>
-    <t>PLO 5</t>
-  </si>
-  <si>
-    <t>PLO 6</t>
-  </si>
-  <si>
-    <t>PLO 7</t>
-  </si>
-  <si>
-    <t>PLO 8</t>
-  </si>
-  <si>
-    <t>PLO 9</t>
-  </si>
-  <si>
-    <t>PLO 10</t>
-  </si>
-  <si>
-    <t>PLO 11</t>
-  </si>
-  <si>
-    <t>PLO 12</t>
+    <t>PLO1</t>
+  </si>
+  <si>
+    <t>PLO2</t>
+  </si>
+  <si>
+    <t>PLO3</t>
+  </si>
+  <si>
+    <t>PLO4</t>
+  </si>
+  <si>
+    <t>PLO5</t>
+  </si>
+  <si>
+    <t>PLO6</t>
+  </si>
+  <si>
+    <t>PLO7</t>
+  </si>
+  <si>
+    <t>PLO8</t>
+  </si>
+  <si>
+    <t>PLO9</t>
+  </si>
+  <si>
+    <t>PLO10</t>
+  </si>
+  <si>
+    <t>PLO11</t>
+  </si>
+  <si>
+    <t>PLO12</t>
+  </si>
+  <si>
+    <t>11ตระหนักและเห็นความจำเป็นของการพัฒนาตนเองอย่างต่อเนื่อง มีการเตรียมตัวเพื่อให้สามารถปฏิบัติงานได้โดยลำพังและสามารถเรียนรู้ตลอดชีพเมื่อมีการเปลี่ยนแปลงทางด้านเทคโนโลยีและวิศวกรรม</t>
+  </si>
+  <si>
+    <t>11Recognize the need for continuous self-development, be prepared for independent work, and engage in lifelong learning in response to technological and engineering changes.</t>
   </si>
 </sst>
 </file>
@@ -513,7 +513,7 @@
   <dimension ref="A1:C13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I16" sqref="I16"/>
+      <selection activeCell="F21" sqref="F21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -531,134 +531,134 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="B2" t="s">
         <v>3</v>
       </c>
       <c r="C2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="B3" t="s">
         <v>4</v>
       </c>
       <c r="C3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="B4" t="s">
         <v>5</v>
       </c>
       <c r="C4" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="B5" t="s">
         <v>6</v>
       </c>
       <c r="C5" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="B6" t="s">
         <v>7</v>
       </c>
       <c r="C6" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="B7" t="s">
         <v>8</v>
       </c>
       <c r="C7" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="B8" t="s">
         <v>9</v>
       </c>
       <c r="C8" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="B9" t="s">
         <v>10</v>
       </c>
       <c r="C9" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="B10" t="s">
         <v>11</v>
       </c>
       <c r="C10" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="B11" t="s">
         <v>12</v>
       </c>
       <c r="C11" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="B12" t="s">
         <v>13</v>
       </c>
       <c r="C12" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
+        <v>36</v>
+      </c>
+      <c r="B13" t="s">
+        <v>37</v>
+      </c>
+      <c r="C13" t="s">
         <v>38</v>
-      </c>
-      <c r="B13" t="s">
-        <v>14</v>
-      </c>
-      <c r="C13" t="s">
-        <v>26</v>
       </c>
     </row>
   </sheetData>

</xml_diff>